<commit_message>
finished link skills, added MATT
</commit_message>
<xml_diff>
--- a/public/mapleaio/equips.xlsx
+++ b/public/mapleaio/equips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VisualStudio\PBWaitingRoom\public\mapleaio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CE7565AC-6443-47CB-BEE2-09967D98E410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCCAC1B8-143E-4A63-AD66-E3B6C376847A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="31800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="71">
   <si>
     <t>name</t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t>MAGE</t>
+  </si>
+  <si>
+    <t>matt</t>
   </si>
 </sst>
 </file>
@@ -1093,10 +1096,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S43"/>
+  <dimension ref="A1:T43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="L54" sqref="L54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,7 +1111,7 @@
     <col min="6" max="6" width="45.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1143,31 +1146,34 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>33</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>34</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1205,14 +1211,14 @@
         <v>0</v>
       </c>
       <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
         <v>30</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>20</v>
       </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
       <c r="P2">
         <v>0</v>
       </c>
@@ -1225,8 +1231,11 @@
       <c r="S2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1261,11 +1270,11 @@
         <v>3</v>
       </c>
       <c r="L3">
+        <v>3</v>
+      </c>
+      <c r="M3">
         <v>300</v>
       </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
       <c r="N3">
         <v>0</v>
       </c>
@@ -1284,8 +1293,11 @@
       <c r="S3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1320,11 +1332,11 @@
         <v>10</v>
       </c>
       <c r="L4">
+        <v>10</v>
+      </c>
+      <c r="M4">
         <v>200</v>
       </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
       <c r="N4">
         <v>0</v>
       </c>
@@ -1343,8 +1355,11 @@
       <c r="S4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1379,7 +1394,7 @@
         <v>77</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -1391,19 +1406,22 @@
         <v>0</v>
       </c>
       <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
         <v>100</v>
       </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
       <c r="R5">
         <v>0</v>
       </c>
       <c r="S5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -1438,11 +1456,11 @@
         <v>3</v>
       </c>
       <c r="L6">
+        <v>3</v>
+      </c>
+      <c r="M6">
         <v>300</v>
       </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
       <c r="N6">
         <v>0</v>
       </c>
@@ -1456,13 +1474,16 @@
         <v>0</v>
       </c>
       <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
         <v>5</v>
       </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1497,7 +1518,7 @@
         <v>10</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -1509,19 +1530,22 @@
         <v>0</v>
       </c>
       <c r="P7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q7">
         <v>100</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="S7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1556,7 +1580,7 @@
         <v>10</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -1568,19 +1592,22 @@
         <v>0</v>
       </c>
       <c r="P8">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q8">
         <v>100</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="S8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -1615,7 +1642,7 @@
         <v>10</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -1627,19 +1654,22 @@
         <v>0</v>
       </c>
       <c r="P9">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q9">
         <v>100</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="S9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -1674,7 +1704,7 @@
         <v>10</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -1686,19 +1716,22 @@
         <v>0</v>
       </c>
       <c r="P10">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q10">
         <v>100</v>
       </c>
       <c r="R10">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="S10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -1733,11 +1766,11 @@
         <v>5</v>
       </c>
       <c r="L11">
+        <v>5</v>
+      </c>
+      <c r="M11">
         <v>100</v>
       </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
       <c r="N11">
         <v>0</v>
       </c>
@@ -1745,19 +1778,22 @@
         <v>0</v>
       </c>
       <c r="P11">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="Q11">
         <v>500</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="S11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -1792,7 +1828,7 @@
         <v>4</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -1804,19 +1840,22 @@
         <v>0</v>
       </c>
       <c r="P12">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="Q12">
         <v>250</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="S12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1851,11 +1890,11 @@
         <v>6</v>
       </c>
       <c r="L13">
+        <v>6</v>
+      </c>
+      <c r="M13">
         <v>150</v>
       </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
       <c r="N13">
         <v>0</v>
       </c>
@@ -1863,19 +1902,22 @@
         <v>0</v>
       </c>
       <c r="P13">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="Q13">
         <v>150</v>
       </c>
       <c r="R13">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="S13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -1910,7 +1952,7 @@
         <v>10</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -1933,8 +1975,11 @@
       <c r="S14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -1969,7 +2014,7 @@
         <v>5</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -1987,13 +2032,16 @@
         <v>0</v>
       </c>
       <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
         <v>700</v>
       </c>
-      <c r="S15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -2028,7 +2076,7 @@
         <v>5</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M16">
         <v>0</v>
@@ -2051,8 +2099,11 @@
       <c r="S16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -2087,7 +2138,7 @@
         <v>5</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M17">
         <v>0</v>
@@ -2105,13 +2156,16 @@
         <v>0</v>
       </c>
       <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
         <v>700</v>
       </c>
-      <c r="S17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -2146,7 +2200,7 @@
         <v>5</v>
       </c>
       <c r="L18">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M18">
         <v>0</v>
@@ -2164,13 +2218,16 @@
         <v>0</v>
       </c>
       <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
         <v>700</v>
       </c>
-      <c r="S18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>66</v>
       </c>
@@ -2205,7 +2262,7 @@
         <v>5</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M19">
         <v>0</v>
@@ -2223,13 +2280,16 @@
         <v>0</v>
       </c>
       <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
         <v>700</v>
       </c>
-      <c r="S19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -2267,14 +2327,14 @@
         <v>0</v>
       </c>
       <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
         <v>30</v>
       </c>
-      <c r="N20">
+      <c r="O20">
         <v>20</v>
       </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
       <c r="P20">
         <v>0</v>
       </c>
@@ -2287,8 +2347,11 @@
       <c r="S20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G21">
         <v>0</v>
       </c>
@@ -2328,8 +2391,11 @@
       <c r="S21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G22">
         <v>0</v>
       </c>
@@ -2369,8 +2435,11 @@
       <c r="S22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G23">
         <v>0</v>
       </c>
@@ -2410,8 +2479,11 @@
       <c r="S23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G24">
         <v>0</v>
       </c>
@@ -2451,8 +2523,11 @@
       <c r="S24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G25">
         <v>0</v>
       </c>
@@ -2492,8 +2567,11 @@
       <c r="S25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G26">
         <v>0</v>
       </c>
@@ -2533,8 +2611,11 @@
       <c r="S26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G27">
         <v>0</v>
       </c>
@@ -2574,8 +2655,11 @@
       <c r="S27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G28">
         <v>0</v>
       </c>
@@ -2615,8 +2699,11 @@
       <c r="S28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G29">
         <v>0</v>
       </c>
@@ -2656,8 +2743,11 @@
       <c r="S29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G30">
         <v>0</v>
       </c>
@@ -2697,8 +2787,11 @@
       <c r="S30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G31">
         <v>0</v>
       </c>
@@ -2738,8 +2831,11 @@
       <c r="S31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G32">
         <v>0</v>
       </c>
@@ -2779,8 +2875,11 @@
       <c r="S32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="T32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G33">
         <v>0</v>
       </c>
@@ -2820,8 +2919,11 @@
       <c r="S33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="T33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G34">
         <v>0</v>
       </c>
@@ -2861,8 +2963,11 @@
       <c r="S34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="T34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G35">
         <v>0</v>
       </c>
@@ -2902,8 +3007,11 @@
       <c r="S35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="T35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G36">
         <v>0</v>
       </c>
@@ -2943,8 +3051,11 @@
       <c r="S36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="T36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G37">
         <v>0</v>
       </c>
@@ -2984,8 +3095,11 @@
       <c r="S37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="T37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G38">
         <v>0</v>
       </c>
@@ -3025,8 +3139,11 @@
       <c r="S38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="T38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G39">
         <v>0</v>
       </c>
@@ -3066,8 +3183,11 @@
       <c r="S39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="T39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G40">
         <v>0</v>
       </c>
@@ -3107,11 +3227,11 @@
       <c r="S40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="P41">
-        <v>0</v>
-      </c>
+      <c r="T40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="7:20" x14ac:dyDescent="0.25">
       <c r="Q41">
         <v>0</v>
       </c>
@@ -3121,11 +3241,11 @@
       <c r="S41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="P42">
-        <v>0</v>
-      </c>
+      <c r="T41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="7:20" x14ac:dyDescent="0.25">
       <c r="Q42">
         <v>0</v>
       </c>
@@ -3135,11 +3255,11 @@
       <c r="S42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="P43">
-        <v>0</v>
-      </c>
+      <c r="T42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="7:20" x14ac:dyDescent="0.25">
       <c r="Q43">
         <v>0</v>
       </c>
@@ -3147,6 +3267,9 @@
         <v>0</v>
       </c>
       <c r="S43">
+        <v>0</v>
+      </c>
+      <c r="T43">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed set bonuses, more data entry
</commit_message>
<xml_diff>
--- a/public/mapleaio/equips.xlsx
+++ b/public/mapleaio/equips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VisualStudio\PBWaitingRoom\public\mapleaio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCCAC1B8-143E-4A63-AD66-E3B6C376847A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A792E13F-27D1-4305-B298-7B6932469046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="31800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="173">
   <si>
     <t>name</t>
   </si>
@@ -233,6 +233,312 @@
   </si>
   <si>
     <t>matt</t>
+  </si>
+  <si>
+    <t>Twilight Mark</t>
+  </si>
+  <si>
+    <t>Daybreak Pendant</t>
+  </si>
+  <si>
+    <t>Estella Earrings</t>
+  </si>
+  <si>
+    <t>Dawn Guardian Angel Ring</t>
+  </si>
+  <si>
+    <t>DAWN</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/a/aa/Eqp_Guardian_Angel_Ring.png</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/4/46/Eqp_Twilight_Mark.png</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/e/e9/Eqp_Daybreak_Pendant.png</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/a/aa/Eqp_Estella_Earrings.png</t>
+  </si>
+  <si>
+    <t>Superior Gollux Ring</t>
+  </si>
+  <si>
+    <t>Superior Engraved Gollux Pendant</t>
+  </si>
+  <si>
+    <t>Superior Engraved Gollux Belt</t>
+  </si>
+  <si>
+    <t>Superior Gollux Earrings</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/9/91/Eqp_Superior_Gollux_Earrings.png/revision/latest?cb=20140829183324</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/4/4c/Eqp_Superior_Engraved_Gollux_Pendant.png/revision/latest?cb=20150922083727</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/6/61/Eqp_Superior_Gollux_Ring.png/revision/latest?cb=20140927222747</t>
+  </si>
+  <si>
+    <t>SUPERIOR_GOLLUX</t>
+  </si>
+  <si>
+    <t>Royal Warrior Helm</t>
+  </si>
+  <si>
+    <t>Eagle Eye Warrior Armor</t>
+  </si>
+  <si>
+    <t>Trixter Warrior Pants</t>
+  </si>
+  <si>
+    <t>HAT</t>
+  </si>
+  <si>
+    <t>TOP</t>
+  </si>
+  <si>
+    <t>BOTTOM</t>
+  </si>
+  <si>
+    <t>RA_WARRIOR</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/a/a1/Eqp_Royal_Warrior_Helm.png/revision/latest?cb=20150112211030</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/5/5e/Eqp_Eagle_Eye_Warrior_Armor.png/revision/latest?cb=20160501235236</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/0/09/Eqp_Trixter_Warrior_Pants.png/revision/latest?cb=20160502025844</t>
+  </si>
+  <si>
+    <t>Royal Dunwitch Helm</t>
+  </si>
+  <si>
+    <t>Eagle Eye Dunwitch Armor</t>
+  </si>
+  <si>
+    <t>Trixter Dunwitch Pants</t>
+  </si>
+  <si>
+    <t>RA_MAGE</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/f/fa/Eqp_Royal_Dunwitch_Hat.png/revision/latest?cb=20141212194412</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/6/69/Eqp_Eagle_Eye_Dunwitch_Robe.png/revision/latest?cb=20160501235242</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/7/79/Eqp_Trixter_Dunwitch_Pants.png/revision/latest?cb=20160502024720</t>
+  </si>
+  <si>
+    <t>Royal Ranger Helm</t>
+  </si>
+  <si>
+    <t>Eagle Eye Ranger Top</t>
+  </si>
+  <si>
+    <t>Trixter Ranger Pants</t>
+  </si>
+  <si>
+    <t>Royal Wanderer Helm</t>
+  </si>
+  <si>
+    <t>Eagle Eye Wanderer Armor</t>
+  </si>
+  <si>
+    <t>Trixter Wanderer Pants</t>
+  </si>
+  <si>
+    <t>RA_BOWMAN</t>
+  </si>
+  <si>
+    <t>RA_PIRATE</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/f/fa/Eqp_Royal_Wanderer_Hat.png/revision/latest?cb=20150112201908</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/8/8c/Eqp_Eagle_Eye_Wanderer_Coat.png/revision/latest?cb=20160501234952</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/e/e0/Eqp_Trixter_Wanderer_Pants.png/revision/latest?cb=20160502022705</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/f/f7/Eqp_Royal_Ranger_Beret.png/revision/latest?cb=20150112211028</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/8/8c/Eqp_Eagle_Eye_Ranger_Cowl.png/revision/latest?cb=20160501234942</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/a/a2/Eqp_Trixter_Ranger_Pants.png/revision/latest?cb=20160502023550</t>
+  </si>
+  <si>
+    <t>Royal Assassin Helm</t>
+  </si>
+  <si>
+    <t>Eagle Eye Assassin Armor</t>
+  </si>
+  <si>
+    <t>Trixter Assassin Pants</t>
+  </si>
+  <si>
+    <t>RA_THIEF</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/8/88/Eqp_Royal_Assassin_Hood.png/revision/latest?cb=20150112211026</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/c/cb/Eqp_Eagle_Eye_Assassin_Shirt.png/revision/latest?cb=20160501234946</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/c/c8/Eqp_Trixter_Assassin_Pants.png/revision/latest?cb=20160502023353</t>
+  </si>
+  <si>
+    <t>Deimos Sage Shield</t>
+  </si>
+  <si>
+    <t>Deimos Shadow Shield</t>
+  </si>
+  <si>
+    <t>Deimos Warrior Shield</t>
+  </si>
+  <si>
+    <t>SECONDARY</t>
+  </si>
+  <si>
+    <t>NO_SET</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/d/d1/Eqp_Deimos_Sage_Shield.png/revision/latest?cb=20180830075149</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/8/80/Eqp_Deimos_Shadow_Shield.png/revision/latest?cb=20180830075204</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/b/b6/Eqp_Deimos_Warrior_Shield.png/revision/latest?cb=20180830075214</t>
+  </si>
+  <si>
+    <t>Princess No's Feather</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/c/cd/Eqp_Princess_No%27s_Feather.png/revision/latest?cb=20170902232433</t>
+  </si>
+  <si>
+    <t>Princess No's Medal</t>
+  </si>
+  <si>
+    <t>Princess No's Flaming Book</t>
+  </si>
+  <si>
+    <t>Princess No's Charm</t>
+  </si>
+  <si>
+    <t>Princess No's Falcon Eye</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/d/dd/Eqp_Princess_No%27s_Falcon_Eye.png/revision/latest?cb=20170903030628</t>
+  </si>
+  <si>
+    <t>https://maplestory.fandom.com/wiki/Princess_No%27s_Flaming_Book</t>
+  </si>
+  <si>
+    <t>https://static.wikiahttps://static.wikia.nocookie.net/maplestory/images/4/44/Eqp_Princess_No%27s_Medal.png/revision/latest?cb=20170902231500.nocookie.net/maplestory/images/c/cd/Eqp_Princess_No%27s_Feather.png/revision/latest?cb=20170902232433</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/4/49/Eqp_Princess_No%27s_Charm.png/revision/latest?cb=20150628094008</t>
+  </si>
+  <si>
+    <t>Arcane Umbra Knight Gloves</t>
+  </si>
+  <si>
+    <t>Arcane Umbra Knight Shoes</t>
+  </si>
+  <si>
+    <t>Arcane Umbra Knight Cape</t>
+  </si>
+  <si>
+    <t>Arcane Umbra Knight Shoulder</t>
+  </si>
+  <si>
+    <t>GLOVES</t>
+  </si>
+  <si>
+    <t>SHOES</t>
+  </si>
+  <si>
+    <t>CAPE</t>
+  </si>
+  <si>
+    <t>SHOULDER</t>
+  </si>
+  <si>
+    <t>ARCANE</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/5/54/Eqp_Arcane_Umbra_Shoes.png/revision/latest?cb=20170122013051</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/6/61/Eqp_Arcane_Umbra_Gloves.png/revision/latest?cb=20170122011728</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/3/3c/Eqp_Arcane_Umbra_Cape.png/revision/latest?cb=20161214031238</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/maplestory/images/b/b8/Eqp_Arcane_Umbra_Shoulder.png/revision/latest?cb=20161209035635</t>
+  </si>
+  <si>
+    <t>Arcane Umbra Archer Gloves</t>
+  </si>
+  <si>
+    <t>Arcane Umbra Archer Shoes</t>
+  </si>
+  <si>
+    <t>Arcane Umbra Archer Cape</t>
+  </si>
+  <si>
+    <t>Arcane Umbra Archer Shoulder</t>
+  </si>
+  <si>
+    <t>Arcane Umbra Pirate Gloves</t>
+  </si>
+  <si>
+    <t>Arcane Umbra Pirate Shoes</t>
+  </si>
+  <si>
+    <t>Arcane Umbra Pirate Cape</t>
+  </si>
+  <si>
+    <t>Arcane Umbra Pirate Shoulder</t>
+  </si>
+  <si>
+    <t>Arcane Umbra Mage Gloves</t>
+  </si>
+  <si>
+    <t>Arcane Umbra Mage Shoes</t>
+  </si>
+  <si>
+    <t>Arcane Umbra Mage Cape</t>
+  </si>
+  <si>
+    <t>Arcane Umbra Mage Shoulder</t>
+  </si>
+  <si>
+    <t>Arcane Umbra Thief Gloves</t>
+  </si>
+  <si>
+    <t>Arcane Umbra Thief Shoes</t>
+  </si>
+  <si>
+    <t>Arcane Umbra Thief Cape</t>
+  </si>
+  <si>
+    <t>Arcane Umbra Thief Shoulder</t>
   </si>
 </sst>
 </file>
@@ -1096,19 +1402,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T43"/>
+  <dimension ref="A1:T72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L54" sqref="L54"/>
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
     <col min="6" max="6" width="45.42578125" customWidth="1"/>
+    <col min="15" max="15" width="8.28515625" customWidth="1"/>
+    <col min="18" max="18" width="6.85546875" customWidth="1"/>
+    <col min="19" max="19" width="5.140625" customWidth="1"/>
+    <col min="20" max="20" width="5.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -2352,26 +2662,44 @@
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21">
+        <v>140</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="G21">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J21">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M21">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N21">
         <v>0</v>
@@ -2396,26 +2724,44 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22">
+        <v>140</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" t="s">
+        <v>75</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G22">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J22">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M22">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N22">
         <v>0</v>
@@ -2433,33 +2779,51 @@
         <v>0</v>
       </c>
       <c r="S22">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T22">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23">
+        <v>160</v>
+      </c>
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="G23">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J23">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M23">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N23">
         <v>0</v>
@@ -2471,10 +2835,10 @@
         <v>0</v>
       </c>
       <c r="Q23">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="R23">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="S23">
         <v>0</v>
@@ -2484,23 +2848,41 @@
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24">
+        <v>160</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" t="s">
+        <v>76</v>
+      </c>
       <c r="G24">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M24">
         <v>0</v>
@@ -2515,10 +2897,10 @@
         <v>0</v>
       </c>
       <c r="Q24">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="R24">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="S24">
         <v>0</v>
@@ -2528,23 +2910,41 @@
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25">
+        <v>160</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" t="s">
+        <v>75</v>
+      </c>
+      <c r="F25" t="s">
+        <v>76</v>
+      </c>
       <c r="G25">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I25">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J25">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M25">
         <v>0</v>
@@ -2559,10 +2959,10 @@
         <v>0</v>
       </c>
       <c r="Q25">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="R25">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="S25">
         <v>0</v>
@@ -2572,26 +2972,44 @@
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26">
+        <v>150</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" t="s">
+        <v>87</v>
+      </c>
+      <c r="F26" t="s">
+        <v>86</v>
+      </c>
       <c r="G26">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J26">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K26">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L26">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M26">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="N26">
         <v>0</v>
@@ -2603,10 +3021,10 @@
         <v>0</v>
       </c>
       <c r="Q26">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="R26">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="S26">
         <v>0</v>
@@ -2616,26 +3034,44 @@
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27">
+        <v>150</v>
+      </c>
+      <c r="C27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" t="s">
+        <v>87</v>
+      </c>
+      <c r="F27" t="s">
+        <v>85</v>
+      </c>
       <c r="G27">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="J27">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="K27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M27">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N27">
         <v>0</v>
@@ -2647,10 +3083,10 @@
         <v>0</v>
       </c>
       <c r="Q27">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="R27">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="S27">
         <v>0</v>
@@ -2660,26 +3096,44 @@
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28">
+        <v>150</v>
+      </c>
+      <c r="C28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" t="s">
+        <v>87</v>
+      </c>
+      <c r="F28" t="s">
+        <v>86</v>
+      </c>
       <c r="G28">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="J28">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="K28">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="L28">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="M28">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N28">
         <v>0</v>
@@ -2691,10 +3145,10 @@
         <v>0</v>
       </c>
       <c r="Q28">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="R28">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="S28">
         <v>0</v>
@@ -2704,26 +3158,44 @@
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29">
+        <v>150</v>
+      </c>
+      <c r="C29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" t="s">
+        <v>87</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="G29">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J29">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K29">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L29">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M29">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N29">
         <v>0</v>
@@ -2735,10 +3207,10 @@
         <v>0</v>
       </c>
       <c r="Q29">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="R29">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="S29">
         <v>0</v>
@@ -2748,11 +3220,29 @@
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30">
+        <v>150</v>
+      </c>
+      <c r="C30" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" t="s">
+        <v>94</v>
+      </c>
+      <c r="F30" t="s">
+        <v>95</v>
+      </c>
       <c r="G30">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="I30">
         <v>0</v>
@@ -2761,28 +3251,28 @@
         <v>0</v>
       </c>
       <c r="K30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L30">
         <v>0</v>
       </c>
       <c r="M30">
-        <v>0</v>
+        <v>390</v>
       </c>
       <c r="N30">
         <v>0</v>
       </c>
       <c r="O30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P30">
         <v>0</v>
       </c>
       <c r="Q30">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="R30">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="S30">
         <v>0</v>
@@ -2792,11 +3282,29 @@
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31">
+        <v>150</v>
+      </c>
+      <c r="C31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" t="s">
+        <v>94</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="G31">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -2805,19 +3313,19 @@
         <v>0</v>
       </c>
       <c r="K31">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L31">
         <v>0</v>
       </c>
       <c r="M31">
-        <v>0</v>
+        <v>210</v>
       </c>
       <c r="N31">
         <v>0</v>
       </c>
       <c r="O31">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P31">
         <v>0</v>
@@ -2836,11 +3344,29 @@
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32">
+        <v>150</v>
+      </c>
+      <c r="C32" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" t="s">
+        <v>94</v>
+      </c>
+      <c r="F32" t="s">
+        <v>97</v>
+      </c>
       <c r="G32">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -2849,19 +3375,19 @@
         <v>0</v>
       </c>
       <c r="K32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L32">
         <v>0</v>
       </c>
       <c r="M32">
-        <v>0</v>
+        <v>210</v>
       </c>
       <c r="N32">
         <v>0</v>
       </c>
       <c r="O32">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P32">
         <v>0</v>
@@ -2879,12 +3405,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33">
+        <v>150</v>
+      </c>
+      <c r="C33" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" t="s">
+        <v>101</v>
+      </c>
+      <c r="F33" t="s">
+        <v>102</v>
+      </c>
       <c r="G33">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="H33">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="I33">
         <v>0</v>
@@ -2893,28 +3437,28 @@
         <v>0</v>
       </c>
       <c r="K33">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L33">
         <v>0</v>
       </c>
       <c r="M33">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="N33">
         <v>0</v>
       </c>
       <c r="O33">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P33">
         <v>0</v>
       </c>
       <c r="Q33">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="R33">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="S33">
         <v>0</v>
@@ -2923,7 +3467,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34">
+        <v>150</v>
+      </c>
+      <c r="C34" t="s">
+        <v>92</v>
+      </c>
+      <c r="D34" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" t="s">
+        <v>101</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G34">
         <v>0</v>
       </c>
@@ -2931,25 +3493,25 @@
         <v>0</v>
       </c>
       <c r="I34">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J34">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K34">
         <v>0</v>
       </c>
       <c r="L34">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M34">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="N34">
         <v>0</v>
       </c>
       <c r="O34">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P34">
         <v>0</v>
@@ -2967,7 +3529,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35">
+        <v>150</v>
+      </c>
+      <c r="C35" t="s">
+        <v>93</v>
+      </c>
+      <c r="D35" t="s">
+        <v>69</v>
+      </c>
+      <c r="E35" t="s">
+        <v>101</v>
+      </c>
+      <c r="F35" t="s">
+        <v>104</v>
+      </c>
       <c r="G35">
         <v>0</v>
       </c>
@@ -2975,25 +3555,25 @@
         <v>0</v>
       </c>
       <c r="I35">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J35">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K35">
         <v>0</v>
       </c>
       <c r="L35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M35">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="N35">
         <v>0</v>
       </c>
       <c r="O35">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P35">
         <v>0</v>
@@ -3011,12 +3591,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36">
+        <v>150</v>
+      </c>
+      <c r="C36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" t="s">
+        <v>67</v>
+      </c>
+      <c r="E36" t="s">
+        <v>111</v>
+      </c>
+      <c r="F36" t="s">
+        <v>116</v>
+      </c>
       <c r="G36">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="H36">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="I36">
         <v>0</v>
@@ -3025,28 +3623,28 @@
         <v>0</v>
       </c>
       <c r="K36">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L36">
         <v>0</v>
       </c>
       <c r="M36">
-        <v>0</v>
+        <v>390</v>
       </c>
       <c r="N36">
         <v>0</v>
       </c>
       <c r="O36">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P36">
         <v>0</v>
       </c>
       <c r="Q36">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="R36">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="S36">
         <v>0</v>
@@ -3055,12 +3653,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37">
+        <v>150</v>
+      </c>
+      <c r="C37" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" t="s">
+        <v>67</v>
+      </c>
+      <c r="E37" t="s">
+        <v>111</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>117</v>
+      </c>
       <c r="G37">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I37">
         <v>0</v>
@@ -3069,19 +3685,19 @@
         <v>0</v>
       </c>
       <c r="K37">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L37">
         <v>0</v>
       </c>
       <c r="M37">
-        <v>0</v>
+        <v>210</v>
       </c>
       <c r="N37">
         <v>0</v>
       </c>
       <c r="O37">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P37">
         <v>0</v>
@@ -3099,12 +3715,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>107</v>
+      </c>
+      <c r="B38">
+        <v>150</v>
+      </c>
+      <c r="C38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" t="s">
+        <v>67</v>
+      </c>
+      <c r="E38" t="s">
+        <v>111</v>
+      </c>
+      <c r="F38" t="s">
+        <v>118</v>
+      </c>
       <c r="G38">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H38">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I38">
         <v>0</v>
@@ -3113,19 +3747,19 @@
         <v>0</v>
       </c>
       <c r="K38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L38">
         <v>0</v>
       </c>
       <c r="M38">
-        <v>0</v>
+        <v>210</v>
       </c>
       <c r="N38">
         <v>0</v>
       </c>
       <c r="O38">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P38">
         <v>0</v>
@@ -3143,12 +3777,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39">
+        <v>150</v>
+      </c>
+      <c r="C39" t="s">
+        <v>91</v>
+      </c>
+      <c r="D39" t="s">
+        <v>68</v>
+      </c>
+      <c r="E39" t="s">
+        <v>112</v>
+      </c>
+      <c r="F39" t="s">
+        <v>113</v>
+      </c>
       <c r="G39">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="I39">
         <v>0</v>
@@ -3157,28 +3809,28 @@
         <v>0</v>
       </c>
       <c r="K39">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L39">
         <v>0</v>
       </c>
       <c r="M39">
-        <v>0</v>
+        <v>390</v>
       </c>
       <c r="N39">
         <v>0</v>
       </c>
       <c r="O39">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P39">
         <v>0</v>
       </c>
       <c r="Q39">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="R39">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="S39">
         <v>0</v>
@@ -3187,12 +3839,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>109</v>
+      </c>
+      <c r="B40">
+        <v>150</v>
+      </c>
+      <c r="C40" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" t="s">
+        <v>68</v>
+      </c>
+      <c r="E40" t="s">
+        <v>112</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="G40">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H40">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I40">
         <v>0</v>
@@ -3201,19 +3871,19 @@
         <v>0</v>
       </c>
       <c r="K40">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L40">
         <v>0</v>
       </c>
       <c r="M40">
-        <v>0</v>
+        <v>210</v>
       </c>
       <c r="N40">
         <v>0</v>
       </c>
       <c r="O40">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P40">
         <v>0</v>
@@ -3231,7 +3901,55 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>110</v>
+      </c>
+      <c r="B41">
+        <v>150</v>
+      </c>
+      <c r="C41" t="s">
+        <v>93</v>
+      </c>
+      <c r="D41" t="s">
+        <v>68</v>
+      </c>
+      <c r="E41" t="s">
+        <v>112</v>
+      </c>
+      <c r="F41" t="s">
+        <v>115</v>
+      </c>
+      <c r="G41">
+        <v>30</v>
+      </c>
+      <c r="H41">
+        <v>30</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>2</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>210</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>5</v>
+      </c>
+      <c r="P41">
+        <v>0</v>
+      </c>
       <c r="Q41">
         <v>0</v>
       </c>
@@ -3245,12 +3963,60 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>119</v>
+      </c>
+      <c r="B42">
+        <v>150</v>
+      </c>
+      <c r="C42" t="s">
+        <v>91</v>
+      </c>
+      <c r="D42" t="s">
+        <v>28</v>
+      </c>
+      <c r="E42" t="s">
+        <v>122</v>
+      </c>
+      <c r="F42" t="s">
+        <v>123</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>40</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>40</v>
+      </c>
+      <c r="K42">
+        <v>2</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>390</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <v>10</v>
+      </c>
+      <c r="P42">
+        <v>0</v>
+      </c>
       <c r="Q42">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="R42">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="S42">
         <v>0</v>
@@ -3259,7 +4025,55 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>120</v>
+      </c>
+      <c r="B43">
+        <v>150</v>
+      </c>
+      <c r="C43" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" t="s">
+        <v>122</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>30</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>30</v>
+      </c>
+      <c r="K43">
+        <v>2</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+      <c r="M43">
+        <v>210</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <v>5</v>
+      </c>
+      <c r="P43">
+        <v>0</v>
+      </c>
       <c r="Q43">
         <v>0</v>
       </c>
@@ -3270,6 +4084,1804 @@
         <v>0</v>
       </c>
       <c r="T43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>121</v>
+      </c>
+      <c r="B44">
+        <v>150</v>
+      </c>
+      <c r="C44" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44" t="s">
+        <v>122</v>
+      </c>
+      <c r="F44" t="s">
+        <v>125</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>30</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>30</v>
+      </c>
+      <c r="K44">
+        <v>2</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>210</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>5</v>
+      </c>
+      <c r="P44">
+        <v>0</v>
+      </c>
+      <c r="Q44">
+        <v>0</v>
+      </c>
+      <c r="R44">
+        <v>0</v>
+      </c>
+      <c r="S44">
+        <v>0</v>
+      </c>
+      <c r="T44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>126</v>
+      </c>
+      <c r="B45">
+        <v>130</v>
+      </c>
+      <c r="C45" t="s">
+        <v>129</v>
+      </c>
+      <c r="D45" t="s">
+        <v>69</v>
+      </c>
+      <c r="E45" t="s">
+        <v>130</v>
+      </c>
+      <c r="F45" t="s">
+        <v>131</v>
+      </c>
+      <c r="G45">
+        <v>10</v>
+      </c>
+      <c r="H45">
+        <v>10</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>118</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <v>0</v>
+      </c>
+      <c r="Q45">
+        <v>0</v>
+      </c>
+      <c r="R45">
+        <v>0</v>
+      </c>
+      <c r="S45">
+        <v>0</v>
+      </c>
+      <c r="T45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>127</v>
+      </c>
+      <c r="B46">
+        <v>130</v>
+      </c>
+      <c r="C46" t="s">
+        <v>129</v>
+      </c>
+      <c r="D46" t="s">
+        <v>28</v>
+      </c>
+      <c r="E46" t="s">
+        <v>130</v>
+      </c>
+      <c r="F46" t="s">
+        <v>132</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>10</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46">
+        <v>0</v>
+      </c>
+      <c r="P46">
+        <v>0</v>
+      </c>
+      <c r="Q46">
+        <v>0</v>
+      </c>
+      <c r="R46">
+        <v>0</v>
+      </c>
+      <c r="S46">
+        <v>0</v>
+      </c>
+      <c r="T46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>128</v>
+      </c>
+      <c r="B47">
+        <v>130</v>
+      </c>
+      <c r="C47" t="s">
+        <v>129</v>
+      </c>
+      <c r="D47" t="s">
+        <v>61</v>
+      </c>
+      <c r="E47" t="s">
+        <v>130</v>
+      </c>
+      <c r="F47" t="s">
+        <v>133</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>10</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+      <c r="O47">
+        <v>0</v>
+      </c>
+      <c r="P47">
+        <v>0</v>
+      </c>
+      <c r="Q47">
+        <v>0</v>
+      </c>
+      <c r="R47">
+        <v>0</v>
+      </c>
+      <c r="S47">
+        <v>0</v>
+      </c>
+      <c r="T47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>136</v>
+      </c>
+      <c r="B48">
+        <v>140</v>
+      </c>
+      <c r="C48" t="s">
+        <v>129</v>
+      </c>
+      <c r="D48" t="s">
+        <v>61</v>
+      </c>
+      <c r="E48" t="s">
+        <v>130</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G48">
+        <v>14</v>
+      </c>
+      <c r="H48">
+        <v>14</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>9</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+      <c r="O48">
+        <v>0</v>
+      </c>
+      <c r="P48">
+        <v>0</v>
+      </c>
+      <c r="Q48">
+        <v>0</v>
+      </c>
+      <c r="R48">
+        <v>0</v>
+      </c>
+      <c r="S48">
+        <v>0</v>
+      </c>
+      <c r="T48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>139</v>
+      </c>
+      <c r="B49">
+        <v>140</v>
+      </c>
+      <c r="C49" t="s">
+        <v>129</v>
+      </c>
+      <c r="D49" t="s">
+        <v>68</v>
+      </c>
+      <c r="E49" t="s">
+        <v>130</v>
+      </c>
+      <c r="F49" t="s">
+        <v>140</v>
+      </c>
+      <c r="G49">
+        <v>14</v>
+      </c>
+      <c r="H49">
+        <v>14</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>9</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
+      <c r="O49">
+        <v>0</v>
+      </c>
+      <c r="P49">
+        <v>0</v>
+      </c>
+      <c r="Q49">
+        <v>0</v>
+      </c>
+      <c r="R49">
+        <v>0</v>
+      </c>
+      <c r="S49">
+        <v>0</v>
+      </c>
+      <c r="T49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>134</v>
+      </c>
+      <c r="B50">
+        <v>140</v>
+      </c>
+      <c r="C50" t="s">
+        <v>129</v>
+      </c>
+      <c r="D50" t="s">
+        <v>67</v>
+      </c>
+      <c r="E50" t="s">
+        <v>130</v>
+      </c>
+      <c r="F50" t="s">
+        <v>135</v>
+      </c>
+      <c r="G50">
+        <v>14</v>
+      </c>
+      <c r="H50">
+        <v>14</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>9</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+      <c r="M50">
+        <v>0</v>
+      </c>
+      <c r="N50">
+        <v>0</v>
+      </c>
+      <c r="O50">
+        <v>0</v>
+      </c>
+      <c r="P50">
+        <v>0</v>
+      </c>
+      <c r="Q50">
+        <v>0</v>
+      </c>
+      <c r="R50">
+        <v>0</v>
+      </c>
+      <c r="S50">
+        <v>0</v>
+      </c>
+      <c r="T50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>138</v>
+      </c>
+      <c r="B51">
+        <v>140</v>
+      </c>
+      <c r="C51" t="s">
+        <v>129</v>
+      </c>
+      <c r="D51" t="s">
+        <v>28</v>
+      </c>
+      <c r="E51" t="s">
+        <v>130</v>
+      </c>
+      <c r="F51" t="s">
+        <v>143</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>14</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>14</v>
+      </c>
+      <c r="K51">
+        <v>9</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <v>0</v>
+      </c>
+      <c r="O51">
+        <v>0</v>
+      </c>
+      <c r="P51">
+        <v>0</v>
+      </c>
+      <c r="Q51">
+        <v>0</v>
+      </c>
+      <c r="R51">
+        <v>0</v>
+      </c>
+      <c r="S51">
+        <v>0</v>
+      </c>
+      <c r="T51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>137</v>
+      </c>
+      <c r="B52">
+        <v>140</v>
+      </c>
+      <c r="C52" t="s">
+        <v>129</v>
+      </c>
+      <c r="D52" t="s">
+        <v>69</v>
+      </c>
+      <c r="E52" t="s">
+        <v>130</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>14</v>
+      </c>
+      <c r="J52">
+        <v>14</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+      <c r="L52">
+        <v>9</v>
+      </c>
+      <c r="M52">
+        <v>0</v>
+      </c>
+      <c r="N52">
+        <v>0</v>
+      </c>
+      <c r="O52">
+        <v>0</v>
+      </c>
+      <c r="P52">
+        <v>0</v>
+      </c>
+      <c r="Q52">
+        <v>0</v>
+      </c>
+      <c r="R52">
+        <v>0</v>
+      </c>
+      <c r="S52">
+        <v>0</v>
+      </c>
+      <c r="T52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>144</v>
+      </c>
+      <c r="B53">
+        <v>200</v>
+      </c>
+      <c r="C53" t="s">
+        <v>148</v>
+      </c>
+      <c r="D53" t="s">
+        <v>61</v>
+      </c>
+      <c r="E53" t="s">
+        <v>152</v>
+      </c>
+      <c r="F53" t="s">
+        <v>154</v>
+      </c>
+      <c r="G53">
+        <v>40</v>
+      </c>
+      <c r="H53">
+        <v>40</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>9</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+      <c r="M53">
+        <v>250</v>
+      </c>
+      <c r="N53">
+        <v>0</v>
+      </c>
+      <c r="O53">
+        <v>0</v>
+      </c>
+      <c r="P53">
+        <v>0</v>
+      </c>
+      <c r="Q53">
+        <v>0</v>
+      </c>
+      <c r="R53">
+        <v>0</v>
+      </c>
+      <c r="S53">
+        <v>0</v>
+      </c>
+      <c r="T53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>145</v>
+      </c>
+      <c r="B54">
+        <v>200</v>
+      </c>
+      <c r="C54" t="s">
+        <v>149</v>
+      </c>
+      <c r="D54" t="s">
+        <v>61</v>
+      </c>
+      <c r="E54" t="s">
+        <v>152</v>
+      </c>
+      <c r="F54" t="s">
+        <v>153</v>
+      </c>
+      <c r="G54">
+        <v>40</v>
+      </c>
+      <c r="H54">
+        <v>40</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>9</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+      <c r="M54">
+        <v>250</v>
+      </c>
+      <c r="N54">
+        <v>0</v>
+      </c>
+      <c r="O54">
+        <v>0</v>
+      </c>
+      <c r="P54">
+        <v>0</v>
+      </c>
+      <c r="Q54">
+        <v>0</v>
+      </c>
+      <c r="R54">
+        <v>0</v>
+      </c>
+      <c r="S54">
+        <v>0</v>
+      </c>
+      <c r="T54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>146</v>
+      </c>
+      <c r="B55">
+        <v>200</v>
+      </c>
+      <c r="C55" t="s">
+        <v>150</v>
+      </c>
+      <c r="D55" t="s">
+        <v>61</v>
+      </c>
+      <c r="E55" t="s">
+        <v>152</v>
+      </c>
+      <c r="F55" t="s">
+        <v>155</v>
+      </c>
+      <c r="G55">
+        <v>35</v>
+      </c>
+      <c r="H55">
+        <v>35</v>
+      </c>
+      <c r="I55">
+        <v>35</v>
+      </c>
+      <c r="J55">
+        <v>35</v>
+      </c>
+      <c r="K55">
+        <v>5</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
+      <c r="M55">
+        <v>450</v>
+      </c>
+      <c r="N55">
+        <v>0</v>
+      </c>
+      <c r="O55">
+        <v>0</v>
+      </c>
+      <c r="P55">
+        <v>0</v>
+      </c>
+      <c r="Q55">
+        <v>0</v>
+      </c>
+      <c r="R55">
+        <v>0</v>
+      </c>
+      <c r="S55">
+        <v>0</v>
+      </c>
+      <c r="T55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>147</v>
+      </c>
+      <c r="B56">
+        <v>200</v>
+      </c>
+      <c r="C56" t="s">
+        <v>151</v>
+      </c>
+      <c r="D56" t="s">
+        <v>61</v>
+      </c>
+      <c r="E56" t="s">
+        <v>152</v>
+      </c>
+      <c r="F56" t="s">
+        <v>156</v>
+      </c>
+      <c r="G56">
+        <v>35</v>
+      </c>
+      <c r="H56">
+        <v>35</v>
+      </c>
+      <c r="I56">
+        <v>35</v>
+      </c>
+      <c r="J56">
+        <v>35</v>
+      </c>
+      <c r="K56">
+        <v>20</v>
+      </c>
+      <c r="L56">
+        <v>0</v>
+      </c>
+      <c r="M56">
+        <v>300</v>
+      </c>
+      <c r="N56">
+        <v>0</v>
+      </c>
+      <c r="O56">
+        <v>0</v>
+      </c>
+      <c r="P56">
+        <v>0</v>
+      </c>
+      <c r="Q56">
+        <v>0</v>
+      </c>
+      <c r="R56">
+        <v>0</v>
+      </c>
+      <c r="S56">
+        <v>0</v>
+      </c>
+      <c r="T56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>157</v>
+      </c>
+      <c r="B57">
+        <v>200</v>
+      </c>
+      <c r="C57" t="s">
+        <v>148</v>
+      </c>
+      <c r="D57" t="s">
+        <v>67</v>
+      </c>
+      <c r="E57" t="s">
+        <v>152</v>
+      </c>
+      <c r="F57" t="s">
+        <v>154</v>
+      </c>
+      <c r="G57">
+        <v>40</v>
+      </c>
+      <c r="H57">
+        <v>40</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>9</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
+      <c r="M57">
+        <v>250</v>
+      </c>
+      <c r="N57">
+        <v>0</v>
+      </c>
+      <c r="O57">
+        <v>0</v>
+      </c>
+      <c r="P57">
+        <v>0</v>
+      </c>
+      <c r="Q57">
+        <v>0</v>
+      </c>
+      <c r="R57">
+        <v>0</v>
+      </c>
+      <c r="S57">
+        <v>0</v>
+      </c>
+      <c r="T57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>158</v>
+      </c>
+      <c r="B58">
+        <v>200</v>
+      </c>
+      <c r="C58" t="s">
+        <v>149</v>
+      </c>
+      <c r="D58" t="s">
+        <v>67</v>
+      </c>
+      <c r="E58" t="s">
+        <v>152</v>
+      </c>
+      <c r="F58" t="s">
+        <v>153</v>
+      </c>
+      <c r="G58">
+        <v>40</v>
+      </c>
+      <c r="H58">
+        <v>40</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <v>9</v>
+      </c>
+      <c r="L58">
+        <v>0</v>
+      </c>
+      <c r="M58">
+        <v>250</v>
+      </c>
+      <c r="N58">
+        <v>0</v>
+      </c>
+      <c r="O58">
+        <v>0</v>
+      </c>
+      <c r="P58">
+        <v>0</v>
+      </c>
+      <c r="Q58">
+        <v>0</v>
+      </c>
+      <c r="R58">
+        <v>0</v>
+      </c>
+      <c r="S58">
+        <v>0</v>
+      </c>
+      <c r="T58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>159</v>
+      </c>
+      <c r="B59">
+        <v>200</v>
+      </c>
+      <c r="C59" t="s">
+        <v>150</v>
+      </c>
+      <c r="D59" t="s">
+        <v>67</v>
+      </c>
+      <c r="E59" t="s">
+        <v>152</v>
+      </c>
+      <c r="F59" t="s">
+        <v>155</v>
+      </c>
+      <c r="G59">
+        <v>35</v>
+      </c>
+      <c r="H59">
+        <v>35</v>
+      </c>
+      <c r="I59">
+        <v>35</v>
+      </c>
+      <c r="J59">
+        <v>35</v>
+      </c>
+      <c r="K59">
+        <v>5</v>
+      </c>
+      <c r="L59">
+        <v>0</v>
+      </c>
+      <c r="M59">
+        <v>450</v>
+      </c>
+      <c r="N59">
+        <v>0</v>
+      </c>
+      <c r="O59">
+        <v>0</v>
+      </c>
+      <c r="P59">
+        <v>0</v>
+      </c>
+      <c r="Q59">
+        <v>0</v>
+      </c>
+      <c r="R59">
+        <v>0</v>
+      </c>
+      <c r="S59">
+        <v>0</v>
+      </c>
+      <c r="T59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>160</v>
+      </c>
+      <c r="B60">
+        <v>200</v>
+      </c>
+      <c r="C60" t="s">
+        <v>151</v>
+      </c>
+      <c r="D60" t="s">
+        <v>67</v>
+      </c>
+      <c r="E60" t="s">
+        <v>152</v>
+      </c>
+      <c r="F60" t="s">
+        <v>156</v>
+      </c>
+      <c r="G60">
+        <v>35</v>
+      </c>
+      <c r="H60">
+        <v>35</v>
+      </c>
+      <c r="I60">
+        <v>35</v>
+      </c>
+      <c r="J60">
+        <v>35</v>
+      </c>
+      <c r="K60">
+        <v>20</v>
+      </c>
+      <c r="L60">
+        <v>0</v>
+      </c>
+      <c r="M60">
+        <v>300</v>
+      </c>
+      <c r="N60">
+        <v>0</v>
+      </c>
+      <c r="O60">
+        <v>0</v>
+      </c>
+      <c r="P60">
+        <v>0</v>
+      </c>
+      <c r="Q60">
+        <v>0</v>
+      </c>
+      <c r="R60">
+        <v>0</v>
+      </c>
+      <c r="S60">
+        <v>0</v>
+      </c>
+      <c r="T60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>161</v>
+      </c>
+      <c r="B61">
+        <v>200</v>
+      </c>
+      <c r="C61" t="s">
+        <v>148</v>
+      </c>
+      <c r="D61" t="s">
+        <v>68</v>
+      </c>
+      <c r="E61" t="s">
+        <v>152</v>
+      </c>
+      <c r="F61" t="s">
+        <v>154</v>
+      </c>
+      <c r="G61">
+        <v>40</v>
+      </c>
+      <c r="H61">
+        <v>40</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+      <c r="K61">
+        <v>9</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
+      <c r="M61">
+        <v>250</v>
+      </c>
+      <c r="N61">
+        <v>0</v>
+      </c>
+      <c r="O61">
+        <v>0</v>
+      </c>
+      <c r="P61">
+        <v>0</v>
+      </c>
+      <c r="Q61">
+        <v>0</v>
+      </c>
+      <c r="R61">
+        <v>0</v>
+      </c>
+      <c r="S61">
+        <v>0</v>
+      </c>
+      <c r="T61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>162</v>
+      </c>
+      <c r="B62">
+        <v>200</v>
+      </c>
+      <c r="C62" t="s">
+        <v>149</v>
+      </c>
+      <c r="D62" t="s">
+        <v>68</v>
+      </c>
+      <c r="E62" t="s">
+        <v>152</v>
+      </c>
+      <c r="F62" t="s">
+        <v>153</v>
+      </c>
+      <c r="G62">
+        <v>40</v>
+      </c>
+      <c r="H62">
+        <v>40</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+      <c r="K62">
+        <v>9</v>
+      </c>
+      <c r="L62">
+        <v>0</v>
+      </c>
+      <c r="M62">
+        <v>250</v>
+      </c>
+      <c r="N62">
+        <v>0</v>
+      </c>
+      <c r="O62">
+        <v>0</v>
+      </c>
+      <c r="P62">
+        <v>0</v>
+      </c>
+      <c r="Q62">
+        <v>0</v>
+      </c>
+      <c r="R62">
+        <v>0</v>
+      </c>
+      <c r="S62">
+        <v>0</v>
+      </c>
+      <c r="T62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>163</v>
+      </c>
+      <c r="B63">
+        <v>200</v>
+      </c>
+      <c r="C63" t="s">
+        <v>150</v>
+      </c>
+      <c r="D63" t="s">
+        <v>68</v>
+      </c>
+      <c r="E63" t="s">
+        <v>152</v>
+      </c>
+      <c r="F63" t="s">
+        <v>155</v>
+      </c>
+      <c r="G63">
+        <v>35</v>
+      </c>
+      <c r="H63">
+        <v>35</v>
+      </c>
+      <c r="I63">
+        <v>35</v>
+      </c>
+      <c r="J63">
+        <v>35</v>
+      </c>
+      <c r="K63">
+        <v>5</v>
+      </c>
+      <c r="L63">
+        <v>0</v>
+      </c>
+      <c r="M63">
+        <v>450</v>
+      </c>
+      <c r="N63">
+        <v>0</v>
+      </c>
+      <c r="O63">
+        <v>0</v>
+      </c>
+      <c r="P63">
+        <v>0</v>
+      </c>
+      <c r="Q63">
+        <v>0</v>
+      </c>
+      <c r="R63">
+        <v>0</v>
+      </c>
+      <c r="S63">
+        <v>0</v>
+      </c>
+      <c r="T63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>164</v>
+      </c>
+      <c r="B64">
+        <v>200</v>
+      </c>
+      <c r="C64" t="s">
+        <v>151</v>
+      </c>
+      <c r="D64" t="s">
+        <v>68</v>
+      </c>
+      <c r="E64" t="s">
+        <v>152</v>
+      </c>
+      <c r="F64" t="s">
+        <v>156</v>
+      </c>
+      <c r="G64">
+        <v>35</v>
+      </c>
+      <c r="H64">
+        <v>35</v>
+      </c>
+      <c r="I64">
+        <v>35</v>
+      </c>
+      <c r="J64">
+        <v>35</v>
+      </c>
+      <c r="K64">
+        <v>20</v>
+      </c>
+      <c r="L64">
+        <v>0</v>
+      </c>
+      <c r="M64">
+        <v>300</v>
+      </c>
+      <c r="N64">
+        <v>0</v>
+      </c>
+      <c r="O64">
+        <v>0</v>
+      </c>
+      <c r="P64">
+        <v>0</v>
+      </c>
+      <c r="Q64">
+        <v>0</v>
+      </c>
+      <c r="R64">
+        <v>0</v>
+      </c>
+      <c r="S64">
+        <v>0</v>
+      </c>
+      <c r="T64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>165</v>
+      </c>
+      <c r="B65">
+        <v>200</v>
+      </c>
+      <c r="C65" t="s">
+        <v>148</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+      <c r="E65" t="s">
+        <v>152</v>
+      </c>
+      <c r="F65" t="s">
+        <v>154</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>40</v>
+      </c>
+      <c r="J65">
+        <v>40</v>
+      </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="L65">
+        <v>9</v>
+      </c>
+      <c r="M65">
+        <v>250</v>
+      </c>
+      <c r="N65">
+        <v>0</v>
+      </c>
+      <c r="O65">
+        <v>0</v>
+      </c>
+      <c r="P65">
+        <v>0</v>
+      </c>
+      <c r="Q65">
+        <v>0</v>
+      </c>
+      <c r="R65">
+        <v>0</v>
+      </c>
+      <c r="S65">
+        <v>0</v>
+      </c>
+      <c r="T65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>166</v>
+      </c>
+      <c r="B66">
+        <v>200</v>
+      </c>
+      <c r="C66" t="s">
+        <v>149</v>
+      </c>
+      <c r="D66" t="s">
+        <v>69</v>
+      </c>
+      <c r="E66" t="s">
+        <v>152</v>
+      </c>
+      <c r="F66" t="s">
+        <v>153</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>40</v>
+      </c>
+      <c r="J66">
+        <v>40</v>
+      </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
+      <c r="L66">
+        <v>9</v>
+      </c>
+      <c r="M66">
+        <v>250</v>
+      </c>
+      <c r="N66">
+        <v>0</v>
+      </c>
+      <c r="O66">
+        <v>0</v>
+      </c>
+      <c r="P66">
+        <v>0</v>
+      </c>
+      <c r="Q66">
+        <v>0</v>
+      </c>
+      <c r="R66">
+        <v>0</v>
+      </c>
+      <c r="S66">
+        <v>0</v>
+      </c>
+      <c r="T66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>167</v>
+      </c>
+      <c r="B67">
+        <v>200</v>
+      </c>
+      <c r="C67" t="s">
+        <v>150</v>
+      </c>
+      <c r="D67" t="s">
+        <v>69</v>
+      </c>
+      <c r="E67" t="s">
+        <v>152</v>
+      </c>
+      <c r="F67" t="s">
+        <v>155</v>
+      </c>
+      <c r="G67">
+        <v>35</v>
+      </c>
+      <c r="H67">
+        <v>35</v>
+      </c>
+      <c r="I67">
+        <v>35</v>
+      </c>
+      <c r="J67">
+        <v>35</v>
+      </c>
+      <c r="K67">
+        <v>0</v>
+      </c>
+      <c r="L67">
+        <v>5</v>
+      </c>
+      <c r="M67">
+        <v>450</v>
+      </c>
+      <c r="N67">
+        <v>0</v>
+      </c>
+      <c r="O67">
+        <v>0</v>
+      </c>
+      <c r="P67">
+        <v>0</v>
+      </c>
+      <c r="Q67">
+        <v>0</v>
+      </c>
+      <c r="R67">
+        <v>0</v>
+      </c>
+      <c r="S67">
+        <v>0</v>
+      </c>
+      <c r="T67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>168</v>
+      </c>
+      <c r="B68">
+        <v>200</v>
+      </c>
+      <c r="C68" t="s">
+        <v>151</v>
+      </c>
+      <c r="D68" t="s">
+        <v>69</v>
+      </c>
+      <c r="E68" t="s">
+        <v>152</v>
+      </c>
+      <c r="F68" t="s">
+        <v>156</v>
+      </c>
+      <c r="G68">
+        <v>35</v>
+      </c>
+      <c r="H68">
+        <v>35</v>
+      </c>
+      <c r="I68">
+        <v>35</v>
+      </c>
+      <c r="J68">
+        <v>35</v>
+      </c>
+      <c r="K68">
+        <v>0</v>
+      </c>
+      <c r="L68">
+        <v>20</v>
+      </c>
+      <c r="M68">
+        <v>300</v>
+      </c>
+      <c r="N68">
+        <v>0</v>
+      </c>
+      <c r="O68">
+        <v>0</v>
+      </c>
+      <c r="P68">
+        <v>0</v>
+      </c>
+      <c r="Q68">
+        <v>0</v>
+      </c>
+      <c r="R68">
+        <v>0</v>
+      </c>
+      <c r="S68">
+        <v>0</v>
+      </c>
+      <c r="T68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>169</v>
+      </c>
+      <c r="B69">
+        <v>200</v>
+      </c>
+      <c r="C69" t="s">
+        <v>148</v>
+      </c>
+      <c r="D69" t="s">
+        <v>28</v>
+      </c>
+      <c r="E69" t="s">
+        <v>152</v>
+      </c>
+      <c r="F69" t="s">
+        <v>154</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>40</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+      <c r="J69">
+        <v>40</v>
+      </c>
+      <c r="K69">
+        <v>9</v>
+      </c>
+      <c r="L69">
+        <v>0</v>
+      </c>
+      <c r="M69">
+        <v>250</v>
+      </c>
+      <c r="N69">
+        <v>0</v>
+      </c>
+      <c r="O69">
+        <v>0</v>
+      </c>
+      <c r="P69">
+        <v>0</v>
+      </c>
+      <c r="Q69">
+        <v>0</v>
+      </c>
+      <c r="R69">
+        <v>0</v>
+      </c>
+      <c r="S69">
+        <v>0</v>
+      </c>
+      <c r="T69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>170</v>
+      </c>
+      <c r="B70">
+        <v>200</v>
+      </c>
+      <c r="C70" t="s">
+        <v>149</v>
+      </c>
+      <c r="D70" t="s">
+        <v>28</v>
+      </c>
+      <c r="E70" t="s">
+        <v>152</v>
+      </c>
+      <c r="F70" t="s">
+        <v>153</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>40</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <v>40</v>
+      </c>
+      <c r="K70">
+        <v>9</v>
+      </c>
+      <c r="L70">
+        <v>0</v>
+      </c>
+      <c r="M70">
+        <v>250</v>
+      </c>
+      <c r="N70">
+        <v>0</v>
+      </c>
+      <c r="O70">
+        <v>0</v>
+      </c>
+      <c r="P70">
+        <v>0</v>
+      </c>
+      <c r="Q70">
+        <v>0</v>
+      </c>
+      <c r="R70">
+        <v>0</v>
+      </c>
+      <c r="S70">
+        <v>0</v>
+      </c>
+      <c r="T70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>171</v>
+      </c>
+      <c r="B71">
+        <v>200</v>
+      </c>
+      <c r="C71" t="s">
+        <v>150</v>
+      </c>
+      <c r="D71" t="s">
+        <v>28</v>
+      </c>
+      <c r="E71" t="s">
+        <v>152</v>
+      </c>
+      <c r="F71" t="s">
+        <v>155</v>
+      </c>
+      <c r="G71">
+        <v>35</v>
+      </c>
+      <c r="H71">
+        <v>35</v>
+      </c>
+      <c r="I71">
+        <v>35</v>
+      </c>
+      <c r="J71">
+        <v>35</v>
+      </c>
+      <c r="K71">
+        <v>5</v>
+      </c>
+      <c r="L71">
+        <v>0</v>
+      </c>
+      <c r="M71">
+        <v>450</v>
+      </c>
+      <c r="N71">
+        <v>0</v>
+      </c>
+      <c r="O71">
+        <v>0</v>
+      </c>
+      <c r="P71">
+        <v>0</v>
+      </c>
+      <c r="Q71">
+        <v>0</v>
+      </c>
+      <c r="R71">
+        <v>0</v>
+      </c>
+      <c r="S71">
+        <v>0</v>
+      </c>
+      <c r="T71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>172</v>
+      </c>
+      <c r="B72">
+        <v>200</v>
+      </c>
+      <c r="C72" t="s">
+        <v>151</v>
+      </c>
+      <c r="D72" t="s">
+        <v>28</v>
+      </c>
+      <c r="E72" t="s">
+        <v>152</v>
+      </c>
+      <c r="F72" t="s">
+        <v>156</v>
+      </c>
+      <c r="G72">
+        <v>35</v>
+      </c>
+      <c r="H72">
+        <v>35</v>
+      </c>
+      <c r="I72">
+        <v>35</v>
+      </c>
+      <c r="J72">
+        <v>35</v>
+      </c>
+      <c r="K72">
+        <v>20</v>
+      </c>
+      <c r="L72">
+        <v>0</v>
+      </c>
+      <c r="M72">
+        <v>300</v>
+      </c>
+      <c r="N72">
+        <v>0</v>
+      </c>
+      <c r="O72">
+        <v>0</v>
+      </c>
+      <c r="P72">
+        <v>0</v>
+      </c>
+      <c r="Q72">
+        <v>0</v>
+      </c>
+      <c r="R72">
+        <v>0</v>
+      </c>
+      <c r="S72">
+        <v>0</v>
+      </c>
+      <c r="T72">
         <v>0</v>
       </c>
     </row>
@@ -3280,8 +5892,21 @@
     <hyperlink ref="F8" r:id="rId3" xr:uid="{DC7DE327-B7DA-48B2-AD74-EB56E5CB0CD1}"/>
     <hyperlink ref="F9" r:id="rId4" xr:uid="{0F1F9638-ED6E-4799-9C2E-527EA26FDB55}"/>
     <hyperlink ref="F10" r:id="rId5" xr:uid="{FBC0EED9-5D5C-4575-A04F-7A7EC53CCECE}"/>
+    <hyperlink ref="F21" r:id="rId6" xr:uid="{22BF0D46-479C-4358-BCF8-C180880426EA}"/>
+    <hyperlink ref="F22" r:id="rId7" xr:uid="{B1443BA5-215C-4014-86BE-7F3006793018}"/>
+    <hyperlink ref="F23" r:id="rId8" xr:uid="{C0FD2424-25F8-49B7-A27A-691AE285B436}"/>
+    <hyperlink ref="F29" r:id="rId9" xr:uid="{33780B2C-2331-40F8-861E-5EC143D60C32}"/>
+    <hyperlink ref="A30" r:id="rId10" tooltip="Royal Warrior Helm" display="https://maplestory.fandom.com/wiki/Royal_Warrior_Helm" xr:uid="{E116CA96-EC25-4D3B-8120-B65E983F2174}"/>
+    <hyperlink ref="F31" r:id="rId11" xr:uid="{6FFFEEA5-8453-477A-B82D-6C19D0769B9A}"/>
+    <hyperlink ref="A33" r:id="rId12" tooltip="Royal Warrior Helm" display="https://maplestory.fandom.com/wiki/Royal_Warrior_Helm" xr:uid="{D58D6B6E-C3CD-492E-BBB6-05545E2E0D27}"/>
+    <hyperlink ref="A36" r:id="rId13" tooltip="Royal Warrior Helm" display="https://maplestory.fandom.com/wiki/Royal_Warrior_Helm" xr:uid="{2B85CD0C-D868-497C-9E93-B0EA2F233F0F}"/>
+    <hyperlink ref="A39" r:id="rId14" tooltip="Royal Warrior Helm" display="https://maplestory.fandom.com/wiki/Royal_Warrior_Helm" xr:uid="{ADA7D784-7D0B-480A-9A6B-0BE61826EC30}"/>
+    <hyperlink ref="F40" r:id="rId15" xr:uid="{70C3A112-73AE-471F-A4DE-A8DD2646BBD6}"/>
+    <hyperlink ref="A42" r:id="rId16" tooltip="Royal Warrior Helm" display="https://maplestory.fandom.com/wiki/Royal_Warrior_Helm" xr:uid="{85A4B43E-C31A-4781-9FC5-B70981C539EE}"/>
+    <hyperlink ref="F43" r:id="rId17" xr:uid="{E59849F4-CFE3-4AED-9D8B-D20387ADC93B}"/>
+    <hyperlink ref="F48" r:id="rId18" xr:uid="{E612818F-043B-4272-9253-E5834841EC84}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>